<commit_message>
Modified CRM to maintain consistency , resolves issue #1
</commit_message>
<xml_diff>
--- a/Assignment2/CrossReferenceMatrix.xlsx
+++ b/Assignment2/CrossReferenceMatrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Academics\2nd year\se\Youtube clone\CSAICSABTeam007\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Academics\2nd year\se\Youtube clone\CSAICSABTeam007\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316156BB-3C04-47FD-9CD2-B8E6753CCCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0540A3-2672-4C3E-9252-A3F5B4A8E085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9102599A-3A96-4FFD-962A-5BD2117DEB19}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>Stakeholder</t>
   </si>
@@ -42,15 +42,9 @@
     <t>URD Topic</t>
   </si>
   <si>
-    <t>NFR</t>
-  </si>
-  <si>
     <t>Performance</t>
   </si>
   <si>
-    <t>Accessibility</t>
-  </si>
-  <si>
     <t>URD Section Number</t>
   </si>
   <si>
@@ -72,18 +66,6 @@
     <t>Test Topics</t>
   </si>
   <si>
-    <t>Content Creator</t>
-  </si>
-  <si>
-    <t>Advertisers</t>
-  </si>
-  <si>
-    <t>Viewer</t>
-  </si>
-  <si>
-    <t>Target User Demographics</t>
-  </si>
-  <si>
     <t>Scalability</t>
   </si>
   <si>
@@ -96,9 +78,6 @@
     <t xml:space="preserve"> Search And Discovery</t>
   </si>
   <si>
-    <t>Video Player Features</t>
-  </si>
-  <si>
     <t>User Interaction</t>
   </si>
   <si>
@@ -108,18 +87,6 @@
     <t>Video Uploading and Management</t>
   </si>
   <si>
-    <t>Live Streaming and Engagement</t>
-  </si>
-  <si>
-    <t>Analytics</t>
-  </si>
-  <si>
-    <t>Advertisements</t>
-  </si>
-  <si>
-    <t>Community Features</t>
-  </si>
-  <si>
     <t>Video Upload and Management</t>
   </si>
   <si>
@@ -138,9 +105,6 @@
     <t>Video Analytics</t>
   </si>
   <si>
-    <t>Monetization and Payment</t>
-  </si>
-  <si>
     <t>Admin Panel</t>
   </si>
   <si>
@@ -159,78 +123,27 @@
     <t>User Registration &amp; Authentication</t>
   </si>
   <si>
-    <t>4.2.3</t>
-  </si>
-  <si>
-    <t>4.2.5</t>
-  </si>
-  <si>
-    <t>4.1.2.1</t>
-  </si>
-  <si>
     <t>Authentication Module</t>
   </si>
   <si>
     <t>Content Discovery Module</t>
   </si>
   <si>
-    <t>4.1.2.3</t>
-  </si>
-  <si>
     <t>Video Interaction Module</t>
   </si>
   <si>
     <t>Content Management Service</t>
   </si>
   <si>
-    <t>4.1.2.2, 4.2.4</t>
-  </si>
-  <si>
     <t>Interaction and Engagement Services</t>
   </si>
   <si>
-    <t>4.2.5.2</t>
-  </si>
-  <si>
     <t>Social Features</t>
   </si>
   <si>
-    <t>4.3.1</t>
-  </si>
-  <si>
     <t>Observability and Monitoring</t>
   </si>
   <si>
-    <t>4.2.3.1</t>
-  </si>
-  <si>
-    <t>Video Processing Service</t>
-  </si>
-  <si>
-    <t>4.4.2</t>
-  </si>
-  <si>
-    <t>Advertising Ecosystem</t>
-  </si>
-  <si>
-    <t>4.4.1</t>
-  </si>
-  <si>
-    <t>Ad Targeting Strategy</t>
-  </si>
-  <si>
-    <t>4.4.3</t>
-  </si>
-  <si>
-    <t>Revenue Generation.</t>
-  </si>
-  <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>Reliability</t>
-  </si>
-  <si>
     <t>Architecture Section</t>
   </si>
   <si>
@@ -249,12 +162,6 @@
     <t>Viewer Features</t>
   </si>
   <si>
-    <t>1.3.3</t>
-  </si>
-  <si>
-    <t>Advertiser Features</t>
-  </si>
-  <si>
     <t>Container Diagrams</t>
   </si>
   <si>
@@ -273,13 +180,52 @@
     <t>Content Creator - View Analytics</t>
   </si>
   <si>
-    <t>Content Creator - Edit Video</t>
-  </si>
-  <si>
-    <t>Content Creator - View Comments</t>
-  </si>
-  <si>
-    <t>Monetize Video</t>
+    <t>Content Creators</t>
+  </si>
+  <si>
+    <t>NFRs</t>
+  </si>
+  <si>
+    <t>Viewers</t>
+  </si>
+  <si>
+    <t>Video Playback</t>
+  </si>
+  <si>
+    <t>3.1.2.1</t>
+  </si>
+  <si>
+    <t>3.1.2.2</t>
+  </si>
+  <si>
+    <t>3.1.2.3</t>
+  </si>
+  <si>
+    <t>3.2.5</t>
+  </si>
+  <si>
+    <t>3.2.5.2</t>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>User -Shares a video</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Security Testing</t>
+  </si>
+  <si>
+    <t>Usability Testing</t>
+  </si>
+  <si>
+    <t>Scalability Testing</t>
   </si>
 </sst>
 </file>
@@ -661,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E1E222-6F39-489C-868A-954950CBC8CD}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,127 +633,133 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>4.0999999999999996</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>3.1</v>
       </c>
       <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
-        <v>69</v>
-      </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J2">
         <v>1.1000000000000001</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
-        <v>4.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>3.4</v>
       </c>
       <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
+      <c r="J3">
+        <v>1.4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D4">
         <v>3.3</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="J4">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -815,31 +767,31 @@
         <v>4.5</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>3.6</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="J5">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -847,66 +799,66 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>3.5</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="J6">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>4.2</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>3.2</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="J8">
-        <v>1.2</v>
+        <v>2.1</v>
       </c>
       <c r="K8" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -914,315 +866,162 @@
         <v>4.8</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>3.7</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="J9">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11">
+        <v>1.2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11">
+        <v>6.2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>3.4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>5.2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>4.2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>1.2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12">
+        <v>6.4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>3.2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>5.3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E13" t="s">
         <v>24</v>
       </c>
-      <c r="D10">
-        <v>3.3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="K10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11">
-        <v>3.6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="F13">
+        <v>1.2</v>
+      </c>
+      <c r="G13" t="s">
         <v>42</v>
       </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11">
-        <v>2.4</v>
-      </c>
-      <c r="K11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>4.7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13">
-        <v>3.8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" t="s">
-        <v>61</v>
+      <c r="H13">
+        <v>6.1</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="J13">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
       <c r="K13" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14">
-        <v>4.8</v>
+        <v>5.4</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>3.7</v>
+        <v>4.3</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>71</v>
+        <v>26</v>
+      </c>
+      <c r="F14">
+        <v>1.2</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" t="s">
-        <v>59</v>
+        <v>42</v>
+      </c>
+      <c r="H14">
+        <v>6.3</v>
       </c>
       <c r="I14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>3.9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" t="s">
-        <v>72</v>
-      </c>
-      <c r="H15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17">
-        <v>1.2</v>
-      </c>
-      <c r="G17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17">
-        <v>7.2</v>
-      </c>
-      <c r="I17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>5.2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18">
-        <v>4.2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18">
-        <v>1.2</v>
-      </c>
-      <c r="G18" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18">
-        <v>7.4</v>
-      </c>
-      <c r="I18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>5.3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19">
-        <v>1.2</v>
-      </c>
-      <c r="G19" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19">
-        <v>7.1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>5.4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20">
-        <v>4.3</v>
-      </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20">
-        <v>1.2</v>
-      </c>
-      <c r="G20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20">
-        <v>7.5</v>
-      </c>
-      <c r="I20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>5.5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21">
-        <v>1.2</v>
-      </c>
-      <c r="G21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21">
-        <v>7.3</v>
-      </c>
-      <c r="I21" t="s">
-        <v>63</v>
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <v>3.3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>